<commit_message>
cleanig up microbia activyt analysis
</commit_message>
<xml_diff>
--- a/data/Flowcyto_data.xlsx
+++ b/data/Flowcyto_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/jeh6121_psu_edu/Documents/Documents/Github/BONCAT_gradients/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{EE88D0E0-D373-444D-95BC-DD1C26FD3A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75D5FD9-B33E-47CC-A750-7B34590E9A93}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{EE88D0E0-D373-444D-95BC-DD1C26FD3A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE7BF48F-AB73-4B27-B4CE-571A51EE5722}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{80963955-D9FB-4053-8965-5540B9B1F3EB}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Fraction</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>Endo</t>
-  </si>
-  <si>
     <t>C6WE</t>
   </si>
   <si>
@@ -213,6 +207,12 @@
   </si>
   <si>
     <t>machine</t>
+  </si>
+  <si>
+    <t>Compartment</t>
+  </si>
+  <si>
+    <t>Root</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -607,60 +607,60 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>44354</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
       </c>
       <c r="I2">
         <v>3.4</v>
@@ -675,33 +675,33 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>44258</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>6</v>
       </c>
       <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
       </c>
       <c r="I3">
         <v>8</v>
@@ -716,33 +716,33 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>44354</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4">
         <v>7.5</v>
@@ -757,33 +757,33 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>44258</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5">
         <v>9.8000000000000007</v>
@@ -798,33 +798,33 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>44254</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6">
         <v>16</v>
@@ -839,33 +839,33 @@
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>44254</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7">
         <v>14.8</v>
@@ -880,33 +880,33 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>44258</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8">
         <v>7.6</v>
@@ -921,33 +921,33 @@
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>44254</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>6</v>
       </c>
       <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
       </c>
       <c r="I9">
         <v>23.6</v>
@@ -962,33 +962,33 @@
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>44347</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
         <v>23</v>
       </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10">
         <v>22.9</v>
@@ -1003,33 +1003,33 @@
         <v>2</v>
       </c>
       <c r="M10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>44347</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11">
         <v>22.8</v>
@@ -1044,33 +1044,33 @@
         <v>3</v>
       </c>
       <c r="M11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>44347</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>9</v>
       </c>
       <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
         <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" t="s">
-        <v>29</v>
       </c>
       <c r="I12">
         <v>19.399999999999999</v>
@@ -1085,33 +1085,33 @@
         <v>3</v>
       </c>
       <c r="M12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1">
         <v>44254</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13">
         <v>18.399999999999999</v>
@@ -1126,33 +1126,33 @@
         <v>5</v>
       </c>
       <c r="M13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1">
         <v>44347</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14">
         <v>18.3</v>
@@ -1167,33 +1167,33 @@
         <v>6</v>
       </c>
       <c r="M14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1">
         <v>44347</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>9</v>
       </c>
       <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
         <v>27</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" t="s">
-        <v>29</v>
       </c>
       <c r="I15">
         <v>31.4</v>
@@ -1208,33 +1208,33 @@
         <v>6</v>
       </c>
       <c r="M15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1">
         <v>44354</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <v>9</v>
       </c>
       <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" t="s">
         <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" t="s">
-        <v>29</v>
       </c>
       <c r="I16">
         <v>6.6</v>
@@ -1249,33 +1249,33 @@
         <v>6</v>
       </c>
       <c r="M16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1">
         <v>44354</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17">
         <v>9</v>
       </c>
       <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s">
         <v>27</v>
-      </c>
-      <c r="F17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" t="s">
-        <v>29</v>
       </c>
       <c r="I17">
         <v>6.2</v>
@@ -1290,33 +1290,33 @@
         <v>6</v>
       </c>
       <c r="M17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1">
         <v>44254</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18">
         <v>26.8</v>
@@ -1331,33 +1331,33 @@
         <v>7</v>
       </c>
       <c r="M18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1">
         <v>44354</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19">
         <v>5</v>
@@ -1372,33 +1372,33 @@
         <v>7</v>
       </c>
       <c r="M19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1">
         <v>44354</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I20">
         <v>43</v>
@@ -1413,33 +1413,33 @@
         <v>9</v>
       </c>
       <c r="M20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1">
         <v>44254</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I21">
         <v>41.8</v>
@@ -1454,33 +1454,33 @@
         <v>11</v>
       </c>
       <c r="M21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1">
         <v>44354</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22">
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22">
         <v>5.9</v>
@@ -1495,33 +1495,33 @@
         <v>12</v>
       </c>
       <c r="M22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1">
         <v>44258</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23">
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -1536,33 +1536,33 @@
         <v>14</v>
       </c>
       <c r="M23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1">
         <v>44258</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24">
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I24">
         <v>24.4</v>
@@ -1577,33 +1577,33 @@
         <v>19</v>
       </c>
       <c r="M24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1">
         <v>44258</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25">
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I25">
         <v>45.6</v>
@@ -1618,33 +1618,33 @@
         <v>33</v>
       </c>
       <c r="M25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="1">
         <v>44254</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I26">
         <v>16.399999999999999</v>
@@ -1659,33 +1659,33 @@
         <v>36</v>
       </c>
       <c r="M26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1">
         <v>44254</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I27">
         <v>20.6</v>
@@ -1700,33 +1700,33 @@
         <v>57</v>
       </c>
       <c r="M27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="1">
         <v>44254</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I28">
         <v>19.2</v>
@@ -1741,33 +1741,33 @@
         <v>123</v>
       </c>
       <c r="M28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" s="1">
         <v>44347</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29">
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I29">
         <v>32.799999999999997</v>
@@ -1782,33 +1782,33 @@
         <v>144</v>
       </c>
       <c r="M29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="1">
         <v>44354</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30">
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I30">
         <v>39.299999999999997</v>
@@ -1823,33 +1823,33 @@
         <v>217</v>
       </c>
       <c r="M30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1">
         <v>44354</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31">
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I31">
         <v>35.4</v>
@@ -1864,33 +1864,33 @@
         <v>287</v>
       </c>
       <c r="M31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" s="1">
         <v>44254</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I32">
         <v>49.6</v>
@@ -1905,33 +1905,33 @@
         <v>365</v>
       </c>
       <c r="M32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1">
         <v>44347</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33">
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I33">
         <v>32</v>
@@ -1946,33 +1946,33 @@
         <v>387</v>
       </c>
       <c r="M33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1">
         <v>44258</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D34">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I34">
         <v>44.8</v>
@@ -1987,33 +1987,33 @@
         <v>455</v>
       </c>
       <c r="M34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" s="1">
         <v>44258</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35">
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I35">
         <v>25.9</v>
@@ -2028,33 +2028,33 @@
         <v>511</v>
       </c>
       <c r="M35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="1">
         <v>44254</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I36">
         <v>26.3</v>
@@ -2069,33 +2069,33 @@
         <v>536</v>
       </c>
       <c r="M36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="1">
         <v>44258</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D37">
         <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F37" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I37">
         <v>21.1</v>
@@ -2110,33 +2110,33 @@
         <v>719</v>
       </c>
       <c r="M37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" s="1">
         <v>44254</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38">
         <v>30.9</v>
@@ -2151,33 +2151,33 @@
         <v>937</v>
       </c>
       <c r="M38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" s="1">
         <v>44258</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39">
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I39">
         <v>62</v>
@@ -2192,7 +2192,7 @@
         <v>1621</v>
       </c>
       <c r="M39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
including cell count data
</commit_message>
<xml_diff>
--- a/data/Flowcyto_data.xlsx
+++ b/data/Flowcyto_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/jeh6121_psu_edu/Documents/Documents/Github/BONCAT_gradients/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="8_{EE88D0E0-D373-444D-95BC-DD1C26FD3A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B4F0F0F-2D94-4F4D-ACD2-B325B846695C}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{EE88D0E0-D373-444D-95BC-DD1C26FD3A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC46D36D-6CBE-4A46-BA3A-CCB9AF9B08F9}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="10272" windowHeight="11976" xr2:uid="{80963955-D9FB-4053-8965-5540B9B1F3EB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{80963955-D9FB-4053-8965-5540B9B1F3EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -588,20 +588,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A70F881-5234-4777-B7FF-60CA1F1CD7E9}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -642,7 +641,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -683,7 +682,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -724,7 +723,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -765,7 +764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -806,7 +805,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -847,7 +846,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -888,7 +887,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -929,7 +928,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -970,7 +969,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1052,7 +1051,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1093,7 +1092,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1134,7 +1133,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1175,7 +1174,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1257,7 +1256,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1298,7 +1297,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1339,7 +1338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1380,7 +1379,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1421,7 +1420,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1462,7 +1461,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1544,7 +1543,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1626,7 +1625,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1667,7 +1666,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1708,7 +1707,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1749,7 +1748,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1831,7 +1830,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1872,7 +1871,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1913,7 +1912,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1954,7 +1953,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1995,7 +1994,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2036,7 +2035,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2077,7 +2076,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2202,18 +2201,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M39" xr:uid="{5A70F881-5234-4777-B7FF-60CA1F1CD7E9}">
-    <filterColumn colId="1">
-      <filters>
-        <dateGroupItem year="2021" month="5" dateTimeGrouping="month"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Bulk"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M39">
-      <sortCondition ref="D1:D39"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M36">
+      <sortCondition ref="F1:F39"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>